<commit_message>
render with aggregate estimates
</commit_message>
<xml_diff>
--- a/Data/Experimental GDP Modelling.xlsx
+++ b/Data/Experimental GDP Modelling.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spulick/GitHub/fa_grants/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\fa_grants\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC2EFD14-47E7-AB49-83AF-13AFEEF06A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03054996-626B-433A-BB28-9FAD497922B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{DAF64436-A789-8F4A-8849-B97D99D9C6B0}"/>
+    <workbookView xWindow="-330" yWindow="-16500" windowWidth="29040" windowHeight="15720" xr2:uid="{DAF64436-A789-8F4A-8849-B97D99D9C6B0}"/>
   </bookViews>
   <sheets>
     <sheet name="GRP" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -207,7 +207,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -263,7 +263,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,21 +622,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B464BD4D-2025-EF4F-BB53-0019258801E7}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="23.84765625" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="24.83203125" customWidth="1"/>
-    <col min="4" max="8" width="16.1640625" customWidth="1"/>
-    <col min="9" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.84765625" customWidth="1"/>
+    <col min="4" max="8" width="16.1484375" customWidth="1"/>
+    <col min="9" max="10" width="22.84765625" customWidth="1"/>
+    <col min="11" max="11" width="17.34765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="36" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -671,7 +671,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -710,7 +710,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -749,7 +749,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -788,7 +788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -866,7 +866,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -905,7 +905,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -944,7 +944,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -983,7 +983,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1061,7 +1061,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>-1.3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1256,10 +1256,10 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.6">
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
         <v>42</v>
       </c>

</xml_diff>